<commit_message>
version_2 is ready this version should be overall faster than the previous
</commit_message>
<xml_diff>
--- a/version_1/version_1.xlsx
+++ b/version_1/version_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\College\Sophomore\Semester 4\CSCI 494-006\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\sebas\parallel-grid-searcher\version_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3A8A14-0EBE-4A34-8C28-1763C92FA9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC10DC63-2C4F-4C27-A073-6BAF64A5E93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parallel_search" sheetId="1" r:id="rId1"/>
@@ -673,7 +673,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -9606,7 +9605,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>485946</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>36737</xdr:rowOff>
+      <xdr:rowOff>110153</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9621,8 +9620,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8850749" y="2585538"/>
-          <a:ext cx="1490656" cy="959898"/>
+          <a:off x="8811872" y="2540181"/>
+          <a:ext cx="1484176" cy="1017115"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9985,7 +9984,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>6545</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>126352</xdr:rowOff>
+      <xdr:rowOff>84235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
@@ -10006,8 +10005,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9862004" y="3635051"/>
-          <a:ext cx="4574462" cy="783513"/>
+          <a:off x="9816647" y="3531378"/>
+          <a:ext cx="4551783" cy="812671"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10625,8 +10624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="N8" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11140,38 +11139,38 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <f>(B2+B8)/2</f>
+        <f t="shared" ref="B14:E17" si="0">(B2+B8)/2</f>
         <v>1345.5</v>
       </c>
       <c r="C14">
-        <f>(C2+C8)/2</f>
+        <f t="shared" si="0"/>
         <v>1122.5</v>
       </c>
       <c r="D14">
-        <f>(D2+D8)/2</f>
+        <f t="shared" si="0"/>
         <v>886</v>
       </c>
       <c r="E14">
-        <f>(E2+E8)/2</f>
+        <f t="shared" si="0"/>
         <v>957</v>
       </c>
       <c r="G14" t="s">
         <v>3</v>
       </c>
       <c r="H14">
-        <f>(H2+H8)/2</f>
+        <f t="shared" ref="H14:K17" si="1">(H2+H8)/2</f>
         <v>431</v>
       </c>
       <c r="I14">
-        <f>(I2+I8)/2</f>
+        <f t="shared" si="1"/>
         <v>570</v>
       </c>
       <c r="J14">
-        <f>(J2+J8)/2</f>
+        <f t="shared" si="1"/>
         <v>373</v>
       </c>
       <c r="K14">
-        <f>(K2+K8)/2</f>
+        <f t="shared" si="1"/>
         <v>388</v>
       </c>
     </row>
@@ -11180,38 +11179,38 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <f>(B3+B9)/2</f>
+        <f t="shared" si="0"/>
         <v>1294.5</v>
       </c>
       <c r="C15">
-        <f>(C3+C9)/2</f>
+        <f t="shared" si="0"/>
         <v>992</v>
       </c>
       <c r="D15">
-        <f>(D3+D9)/2</f>
+        <f t="shared" si="0"/>
         <v>570</v>
       </c>
       <c r="E15">
-        <f>(E3+E9)/2</f>
+        <f t="shared" si="0"/>
         <v>527</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
       </c>
       <c r="H15">
-        <f>(H3+H9)/2</f>
+        <f t="shared" si="1"/>
         <v>470.5</v>
       </c>
       <c r="I15">
-        <f>(I3+I9)/2</f>
+        <f t="shared" si="1"/>
         <v>562.5</v>
       </c>
       <c r="J15">
-        <f>(J3+J9)/2</f>
+        <f t="shared" si="1"/>
         <v>364.5</v>
       </c>
       <c r="K15">
-        <f>(K3+K9)/2</f>
+        <f t="shared" si="1"/>
         <v>380.5</v>
       </c>
       <c r="M15" t="s">
@@ -11226,38 +11225,38 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <f>(B4+B10)/2</f>
+        <f t="shared" si="0"/>
         <v>1269.5</v>
       </c>
       <c r="C16">
-        <f>(C4+C10)/2</f>
+        <f t="shared" si="0"/>
         <v>965.5</v>
       </c>
       <c r="D16">
-        <f>(D4+D10)/2</f>
+        <f t="shared" si="0"/>
         <v>564.5</v>
       </c>
       <c r="E16">
-        <f>(E4+E10)/2</f>
+        <f t="shared" si="0"/>
         <v>421</v>
       </c>
       <c r="G16" t="s">
         <v>17</v>
       </c>
       <c r="H16">
-        <f>(H4+H10)/2</f>
+        <f t="shared" si="1"/>
         <v>401.5</v>
       </c>
       <c r="I16">
-        <f>(I4+I10)/2</f>
+        <f t="shared" si="1"/>
         <v>553.5</v>
       </c>
       <c r="J16">
-        <f>(J4+J10)/2</f>
+        <f t="shared" si="1"/>
         <v>365</v>
       </c>
       <c r="K16">
-        <f>(K4+K10)/2</f>
+        <f t="shared" si="1"/>
         <v>375</v>
       </c>
       <c r="M16" t="s">
@@ -11273,38 +11272,38 @@
         <v>3</v>
       </c>
       <c r="B17">
-        <f>(B5+B11)/2</f>
+        <f t="shared" si="0"/>
         <v>1277</v>
       </c>
       <c r="C17">
-        <f>(C5+C11)/2</f>
+        <f t="shared" si="0"/>
         <v>950</v>
       </c>
       <c r="D17">
-        <f>(D5+D11)/2</f>
+        <f t="shared" si="0"/>
         <v>612</v>
       </c>
       <c r="E17">
-        <f>(E5+E11)/2</f>
+        <f t="shared" si="0"/>
         <v>427.5</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
       </c>
       <c r="H17">
-        <f>(H5+H11)/2</f>
+        <f t="shared" si="1"/>
         <v>389</v>
       </c>
       <c r="I17">
-        <f>(I5+I11)/2</f>
+        <f t="shared" si="1"/>
         <v>544</v>
       </c>
       <c r="J17">
-        <f>(J5+J11)/2</f>
+        <f t="shared" si="1"/>
         <v>360</v>
       </c>
       <c r="K17">
-        <f>(K5+K11)/2</f>
+        <f t="shared" si="1"/>
         <v>389</v>
       </c>
       <c r="M17" t="s">

</xml_diff>